<commit_message>
Progress on longform evaluation, st detection & simplification
</commit_message>
<xml_diff>
--- a/inst/models/checkimab/model.xlsx
+++ b/inst/models/checkimab/model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanamdahl/Documents/R/R-Packages/heRomod2/inst/models/checkimab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858353E4-67B8-0246-8EE2-70FCC937B0C0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637666DD-E130-7246-A01F-3361508B6D6D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15960" activeTab="5" xr2:uid="{F2154858-BAC7-AB46-9308-23215F5D2873}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{F2154858-BAC7-AB46-9308-23215F5D2873}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="126">
   <si>
     <t>timeframe</t>
   </si>
@@ -5550,8 +5550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{256F5870-E244-6849-9316-9568A14419E4}">
   <dimension ref="A1:H569"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C2" zoomScale="143" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12009,15 +12009,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E385199-510B-2B49-B477-B59AC0B6C5BF}">
   <dimension ref="A1:F834"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="25.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="25.5" style="9" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" style="9" customWidth="1"/>
     <col min="3" max="3" width="36.1640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="85.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.6640625" style="9" customWidth="1"/>
     <col min="5" max="5" width="36.1640625" style="9" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="9"/>
   </cols>
@@ -12046,7 +12047,7 @@
       <c r="C2" t="s">
         <v>73</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="20" t="s">
         <v>122</v>
       </c>
     </row>
@@ -12088,39 +12089,75 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
+      <c r="B6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
+      <c r="B7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="20">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
+      <c r="B8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="20">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="20">
+        <v>0.04</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11"/>
-      <c r="D11"/>
+      <c r="B11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="20">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12"/>

</xml_diff>

<commit_message>
Moved trees onto standardized evaluation framework.
</commit_message>
<xml_diff>
--- a/inst/models/checkimab/model.xlsx
+++ b/inst/models/checkimab/model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanamdahl/Documents/R/R-Packages/heRomod2/inst/models/checkimab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D346AEC0-762E-DF41-9F73-07A8B3A939C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF2887F-2F58-7B41-945D-1337ABACF4F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{F2154858-BAC7-AB46-9308-23215F5D2873}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15960" activeTab="1" xr2:uid="{F2154858-BAC7-AB46-9308-23215F5D2873}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="147">
   <si>
     <t>timeframe</t>
   </si>
@@ -473,6 +473,15 @@
   </si>
   <si>
     <t>share_state_time</t>
+  </si>
+  <si>
+    <t>normal(bc, bc * 0.25)</t>
+  </si>
+  <si>
+    <t>cost_nausea</t>
+  </si>
+  <si>
+    <t>Nausea, Cost per Event</t>
   </si>
 </sst>
 </file>
@@ -2410,8 +2419,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A864B13E-9722-6C40-BC17-06B0EC44FC76}" name="Table1" displayName="Table1" ref="A1:H569" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72" tableBorderDxfId="71">
-  <autoFilter ref="A1:H569" xr:uid="{3D81EAC8-05DA-D049-B501-1CD472FC6154}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A864B13E-9722-6C40-BC17-06B0EC44FC76}" name="Table1" displayName="Table1" ref="A1:H570" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72" tableBorderDxfId="71">
+  <autoFilter ref="A1:H570" xr:uid="{3D81EAC8-05DA-D049-B501-1CD472FC6154}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{C5331D5E-A656-7D47-8018-7642F10E6CA8}" name="name" dataDxfId="70"/>
     <tableColumn id="2" xr3:uid="{FEA74BC7-2D0A-FF42-8C35-D063305661C6}" name="display_name" dataDxfId="69"/>
@@ -5640,10 +5649,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{256F5870-E244-6849-9316-9568A14419E4}">
-  <dimension ref="A1:H569"/>
+  <dimension ref="A1:H570"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5702,7 +5711,9 @@
       <c r="F2" s="20">
         <v>26</v>
       </c>
-      <c r="G2" s="20"/>
+      <c r="G2" s="20" t="s">
+        <v>144</v>
+      </c>
       <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -5722,7 +5733,9 @@
       <c r="F3" s="20">
         <v>45</v>
       </c>
-      <c r="G3" s="20"/>
+      <c r="G3" s="20" t="s">
+        <v>144</v>
+      </c>
       <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -5742,7 +5755,9 @@
       <c r="F4" s="20">
         <v>27</v>
       </c>
-      <c r="G4" s="20"/>
+      <c r="G4" s="20" t="s">
+        <v>144</v>
+      </c>
       <c r="H4" s="18"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -5762,7 +5777,9 @@
       <c r="F5" s="20">
         <v>48</v>
       </c>
-      <c r="G5" s="20"/>
+      <c r="G5" s="20" t="s">
+        <v>144</v>
+      </c>
       <c r="H5" s="18"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -5898,7 +5915,9 @@
       <c r="F12" s="20">
         <v>1E-3</v>
       </c>
-      <c r="G12" s="20"/>
+      <c r="G12" s="20" t="s">
+        <v>144</v>
+      </c>
       <c r="H12" s="18"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -5918,7 +5937,9 @@
       <c r="F13" s="20">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="G13" s="20"/>
+      <c r="G13" s="20" t="s">
+        <v>144</v>
+      </c>
       <c r="H13" s="18"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -5938,27 +5959,29 @@
       <c r="F14" s="20">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="G14" s="20"/>
+      <c r="G14" s="20" t="s">
+        <v>144</v>
+      </c>
       <c r="H14" s="18"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="D15" t="s">
-        <v>62</v>
-      </c>
+      <c r="A15" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D15" s="15"/>
       <c r="E15" s="18"/>
-      <c r="F15" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="G15" s="20"/>
+      <c r="F15" s="15">
+        <v>1000</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>144</v>
+      </c>
       <c r="H15" s="18"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -5972,11 +5995,11 @@
         <v>93</v>
       </c>
       <c r="D16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E16" s="18"/>
       <c r="F16" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G16" s="20"/>
       <c r="H16" s="18"/>
@@ -5992,31 +6015,31 @@
         <v>93</v>
       </c>
       <c r="D17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E17" s="18"/>
       <c r="F17" s="20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G17" s="20"/>
       <c r="H17" s="18"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="20" t="s">
-        <v>48</v>
+      <c r="A18" s="16" t="s">
+        <v>47</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E18" s="18"/>
       <c r="F18" s="20" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="G18" s="20"/>
       <c r="H18" s="18"/>
@@ -6032,11 +6055,11 @@
         <v>95</v>
       </c>
       <c r="D19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E19" s="18"/>
       <c r="F19" s="20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G19" s="20"/>
       <c r="H19" s="18"/>
@@ -6052,94 +6075,104 @@
         <v>95</v>
       </c>
       <c r="D20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E20" s="18"/>
       <c r="F20" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G20" s="20"/>
       <c r="H20" s="18"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
-        <v>100</v>
+        <v>48</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="D21" s="18"/>
+        <v>95</v>
+      </c>
+      <c r="D21" t="s">
+        <v>64</v>
+      </c>
       <c r="E21" s="18"/>
       <c r="F21" s="20" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="G21" s="20"/>
       <c r="H21" s="18"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D22" s="18"/>
       <c r="E22" s="18"/>
       <c r="F22" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G22" s="20"/>
       <c r="H22" s="18"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
       <c r="F23" s="20" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="G23" s="20"/>
       <c r="H23" s="18"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
-        <v>137</v>
+        <v>106</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>138</v>
+        <v>107</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>138</v>
+        <v>107</v>
       </c>
       <c r="D24" s="18"/>
       <c r="E24" s="18"/>
       <c r="F24" s="20" t="s">
-        <v>139</v>
+        <v>112</v>
       </c>
       <c r="G24" s="20"/>
       <c r="H24" s="18"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="20"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
+      <c r="A25" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>138</v>
+      </c>
       <c r="D25" s="18"/>
       <c r="E25" s="18"/>
-      <c r="F25" s="20"/>
+      <c r="F25" s="20" t="s">
+        <v>139</v>
+      </c>
       <c r="G25" s="20"/>
       <c r="H25" s="18"/>
     </row>
@@ -6159,7 +6192,7 @@
       <c r="C27" s="20"/>
       <c r="D27" s="18"/>
       <c r="E27" s="18"/>
-      <c r="F27" s="16"/>
+      <c r="F27" s="20"/>
       <c r="G27" s="20"/>
       <c r="H27" s="18"/>
     </row>
@@ -6199,7 +6232,7 @@
       <c r="C31" s="20"/>
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
-      <c r="F31" s="20"/>
+      <c r="F31" s="16"/>
       <c r="G31" s="20"/>
       <c r="H31" s="18"/>
     </row>
@@ -6918,10 +6951,10 @@
       <c r="B103" s="20"/>
       <c r="C103" s="20"/>
       <c r="D103" s="18"/>
-      <c r="E103" s="15"/>
+      <c r="E103" s="18"/>
       <c r="F103" s="20"/>
       <c r="G103" s="20"/>
-      <c r="H103" s="15"/>
+      <c r="H103" s="18"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="20"/>
@@ -11274,12 +11307,12 @@
       <c r="H538" s="15"/>
     </row>
     <row r="539" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A539" s="15"/>
-      <c r="B539" s="15"/>
-      <c r="C539" s="15"/>
-      <c r="D539" s="20"/>
-      <c r="E539" s="20"/>
-      <c r="F539" s="15"/>
+      <c r="A539" s="20"/>
+      <c r="B539" s="20"/>
+      <c r="C539" s="20"/>
+      <c r="D539" s="18"/>
+      <c r="E539" s="15"/>
+      <c r="F539" s="20"/>
       <c r="G539" s="20"/>
       <c r="H539" s="15"/>
     </row>
@@ -11427,8 +11460,8 @@
       <c r="A554" s="15"/>
       <c r="B554" s="15"/>
       <c r="C554" s="15"/>
-      <c r="D554" s="15"/>
-      <c r="E554" s="15"/>
+      <c r="D554" s="20"/>
+      <c r="E554" s="20"/>
       <c r="F554" s="15"/>
       <c r="G554" s="20"/>
       <c r="H554" s="15"/>
@@ -11437,7 +11470,7 @@
       <c r="A555" s="15"/>
       <c r="B555" s="15"/>
       <c r="C555" s="15"/>
-      <c r="D555" s="20"/>
+      <c r="D555" s="15"/>
       <c r="E555" s="15"/>
       <c r="F555" s="15"/>
       <c r="G555" s="20"/>
@@ -11582,6 +11615,16 @@
       <c r="F569" s="15"/>
       <c r="G569" s="20"/>
       <c r="H569" s="15"/>
+    </row>
+    <row r="570" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A570" s="15"/>
+      <c r="B570" s="15"/>
+      <c r="C570" s="15"/>
+      <c r="D570" s="20"/>
+      <c r="E570" s="15"/>
+      <c r="F570" s="15"/>
+      <c r="G570" s="20"/>
+      <c r="H570" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11825,8 +11868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24C4CBAC-B29D-6645-89C8-9E5B5D8E4D46}">
   <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E4"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added minimal testing of bootstrapping.
</commit_message>
<xml_diff>
--- a/inst/models/checkimab/model.xlsx
+++ b/inst/models/checkimab/model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanamdahl/Documents/R/R-Packages/heRomod2/inst/models/checkimab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF2887F-2F58-7B41-945D-1337ABACF4F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30DF811F-1163-C84E-83AA-66656245958D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15960" activeTab="1" xr2:uid="{F2154858-BAC7-AB46-9308-23215F5D2873}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{F2154858-BAC7-AB46-9308-23215F5D2873}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="154">
   <si>
     <t>timeframe</t>
   </si>
@@ -482,6 +484,27 @@
   </si>
   <si>
     <t>Nausea, Cost per Event</t>
+  </si>
+  <si>
+    <t>eq5d_model</t>
+  </si>
+  <si>
+    <t>EQ-5D linear model</t>
+  </si>
+  <si>
+    <t>eq5d_data</t>
+  </si>
+  <si>
+    <t>EQ-5D data</t>
+  </si>
+  <si>
+    <t>eq5d</t>
+  </si>
+  <si>
+    <t>bootstrap(bc, id = "id", strata = "treatment")</t>
+  </si>
+  <si>
+    <t>lm(value~treatment+state, data = eq5d_data)</t>
   </si>
 </sst>
 </file>
@@ -5651,8 +5674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{256F5870-E244-6849-9316-9568A14419E4}">
   <dimension ref="A1:H570"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5663,7 +5686,7 @@
     <col min="4" max="4" width="22.1640625" style="9" customWidth="1"/>
     <col min="5" max="5" width="20.33203125" style="9" customWidth="1"/>
     <col min="6" max="6" width="58.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.1640625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="38.5" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="40" style="9" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="9"/>
   </cols>
@@ -6177,22 +6200,40 @@
       <c r="H25" s="18"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="20"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
+      <c r="A26" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>150</v>
+      </c>
       <c r="D26" s="18"/>
       <c r="E26" s="18"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
+      <c r="F26" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>152</v>
+      </c>
       <c r="H26" s="18"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="20"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
+      <c r="A27" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>148</v>
+      </c>
       <c r="D27" s="18"/>
       <c r="E27" s="18"/>
-      <c r="F27" s="20"/>
+      <c r="F27" s="20" t="s">
+        <v>153</v>
+      </c>
       <c r="G27" s="20"/>
       <c r="H27" s="18"/>
     </row>

</xml_diff>

<commit_message>
Added multy type version of outcome function and updated model with added health_value$type
</commit_message>
<xml_diff>
--- a/inst/models/checkimab/model.xlsx
+++ b/inst/models/checkimab/model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexander_lonshteyn/Desktop/HeRomod2/heRomod2/inst/models/checkimab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5EECA7-722B-814C-BDF1-BD31CBD9296F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E85240E-D006-094B-864C-FA47109FE762}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="820" windowWidth="22240" windowHeight="13580" activeTab="5" xr2:uid="{F2154858-BAC7-AB46-9308-23215F5D2873}"/>
+    <workbookView xWindow="1440" yWindow="740" windowWidth="22240" windowHeight="13580" activeTab="6" xr2:uid="{F2154858-BAC7-AB46-9308-23215F5D2873}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="159">
   <si>
     <t>timeframe</t>
   </si>
@@ -503,6 +503,15 @@
   </si>
   <si>
     <t>ifelse(state_cycle &gt; 3, 0.3, 0.3)</t>
+  </si>
+  <si>
+    <t>lifetable</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>end</t>
   </si>
 </sst>
 </file>
@@ -2513,13 +2522,14 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{ECAEE805-6565-A54F-9DEE-3F776EC12FFC}" name="Table17" displayName="Table17" ref="A1:E305" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37" tableBorderDxfId="36">
-  <autoFilter ref="A1:E305" xr:uid="{3D81EAC8-05DA-D049-B501-1CD472FC6154}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{ECAEE805-6565-A54F-9DEE-3F776EC12FFC}" name="Table17" displayName="Table17" ref="A1:F305" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37" tableBorderDxfId="36">
+  <autoFilter ref="A1:F305" xr:uid="{3D81EAC8-05DA-D049-B501-1CD472FC6154}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B672616B-5AD7-C04F-85D1-A80CD6C05684}" name="name" dataDxfId="35"/>
     <tableColumn id="2" xr3:uid="{9359D359-E665-004E-AFAA-ED095E5901BE}" name="display_name" dataDxfId="34"/>
     <tableColumn id="3" xr3:uid="{81785362-73A1-9448-94BF-3672160AD33A}" name="description" dataDxfId="33"/>
     <tableColumn id="5" xr3:uid="{C60112EB-A39D-9044-AA87-C45800C17C3E}" name="state"/>
+    <tableColumn id="6" xr3:uid="{950C716D-738D-CC43-ACE5-DDF27862399B}" name="type"/>
     <tableColumn id="4" xr3:uid="{F2BEAA99-68A5-0A43-AAFE-628903802CE7}" name="formula" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -12219,7 +12229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E385199-510B-2B49-B477-B59AC0B6C5BF}">
   <dimension ref="A1:E834"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -16480,10 +16490,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F0D78FB-8401-9E4C-9EB5-A7C336F3C948}">
-  <dimension ref="A1:E305"/>
+  <dimension ref="A1:F305"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16491,12 +16501,12 @@
     <col min="1" max="1" width="21.33203125" style="9" customWidth="1"/>
     <col min="2" max="2" width="23.83203125" style="9" customWidth="1"/>
     <col min="3" max="3" width="43.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.33203125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="89" style="9" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="9"/>
+    <col min="4" max="5" width="35.33203125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="89" style="9" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
@@ -16510,10 +16520,13 @@
         <v>129</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>130</v>
       </c>
@@ -16526,11 +16539,14 @@
       <c r="D2" t="s">
         <v>68</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>130</v>
       </c>
@@ -16543,11 +16559,14 @@
       <c r="D3" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>130</v>
       </c>
@@ -16560,11 +16579,14 @@
       <c r="D4" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" t="s">
+        <v>157</v>
+      </c>
+      <c r="F4" s="12" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>134</v>
       </c>
@@ -16577,11 +16599,14 @@
       <c r="D5" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F5" s="20" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>134</v>
       </c>
@@ -16594,11 +16619,14 @@
       <c r="D6" t="s">
         <v>69</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" t="s">
+        <v>156</v>
+      </c>
+      <c r="F6" s="20" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>134</v>
       </c>
@@ -16611,2095 +16639,2396 @@
       <c r="D7" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
+        <v>156</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8"/>
       <c r="D8"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E8"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9"/>
       <c r="D9"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E9"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10"/>
       <c r="D10"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E10"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
       <c r="D11"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E11"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
       <c r="D12"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E12"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
       <c r="D13"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E13"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14"/>
       <c r="D14"/>
       <c r="E14"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
       <c r="D15"/>
       <c r="E15"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
       <c r="D17"/>
       <c r="E17"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18"/>
       <c r="E18"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19"/>
       <c r="D19"/>
       <c r="E19"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
       <c r="E21"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
       <c r="D22"/>
       <c r="E22"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
       <c r="D23"/>
       <c r="E23"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
       <c r="D25"/>
       <c r="E25"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
       <c r="D26"/>
       <c r="E26"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
       <c r="E29"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30"/>
       <c r="D30"/>
       <c r="E30"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31"/>
       <c r="D31"/>
       <c r="E31"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32"/>
       <c r="B32"/>
       <c r="C32"/>
       <c r="D32"/>
       <c r="E32"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33"/>
       <c r="B33"/>
       <c r="C33"/>
       <c r="D33"/>
       <c r="E33"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34"/>
       <c r="B34"/>
       <c r="C34"/>
       <c r="D34"/>
       <c r="E34"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35"/>
       <c r="B35"/>
       <c r="C35"/>
       <c r="D35"/>
       <c r="E35"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36"/>
       <c r="B36"/>
       <c r="C36"/>
       <c r="D36"/>
       <c r="E36"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37"/>
       <c r="B37"/>
       <c r="C37"/>
       <c r="D37"/>
       <c r="E37"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38"/>
       <c r="B38"/>
       <c r="C38"/>
       <c r="D38"/>
       <c r="E38"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39"/>
       <c r="B39"/>
       <c r="C39"/>
       <c r="D39"/>
       <c r="E39"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40"/>
       <c r="B40"/>
       <c r="C40"/>
       <c r="D40"/>
       <c r="E40"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41"/>
       <c r="B41"/>
       <c r="C41"/>
       <c r="D41"/>
       <c r="E41"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42"/>
       <c r="B42"/>
       <c r="C42"/>
       <c r="D42"/>
       <c r="E42"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43"/>
       <c r="B43"/>
       <c r="C43"/>
       <c r="D43"/>
       <c r="E43"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44"/>
       <c r="B44"/>
       <c r="C44"/>
       <c r="D44"/>
       <c r="E44"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45"/>
       <c r="B45"/>
       <c r="C45"/>
       <c r="D45"/>
       <c r="E45"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46"/>
       <c r="B46"/>
       <c r="C46"/>
       <c r="D46"/>
       <c r="E46"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47"/>
       <c r="B47"/>
       <c r="C47"/>
       <c r="D47"/>
       <c r="E47"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48"/>
       <c r="B48"/>
       <c r="C48"/>
       <c r="D48"/>
       <c r="E48"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49"/>
       <c r="B49"/>
       <c r="C49"/>
       <c r="D49"/>
       <c r="E49"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50"/>
       <c r="B50"/>
       <c r="C50"/>
       <c r="D50"/>
       <c r="E50"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51"/>
       <c r="B51"/>
       <c r="C51"/>
       <c r="D51"/>
       <c r="E51"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52"/>
       <c r="B52"/>
       <c r="C52"/>
       <c r="D52"/>
       <c r="E52"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53"/>
       <c r="B53"/>
       <c r="C53"/>
       <c r="D53"/>
       <c r="E53"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54"/>
       <c r="B54"/>
       <c r="C54"/>
       <c r="D54"/>
       <c r="E54"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55"/>
       <c r="B55"/>
       <c r="C55"/>
       <c r="D55"/>
       <c r="E55"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56"/>
       <c r="B56"/>
       <c r="C56"/>
       <c r="D56"/>
       <c r="E56"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57"/>
       <c r="B57"/>
       <c r="C57"/>
       <c r="D57"/>
       <c r="E57"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58"/>
       <c r="B58"/>
       <c r="C58"/>
       <c r="D58"/>
       <c r="E58"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59"/>
       <c r="B59"/>
       <c r="C59"/>
       <c r="D59"/>
       <c r="E59"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60"/>
       <c r="B60"/>
       <c r="C60"/>
       <c r="D60"/>
       <c r="E60"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61"/>
       <c r="B61"/>
       <c r="C61"/>
       <c r="D61"/>
       <c r="E61"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62"/>
       <c r="B62"/>
       <c r="C62"/>
       <c r="D62"/>
       <c r="E62"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63"/>
       <c r="B63"/>
       <c r="C63"/>
       <c r="D63"/>
       <c r="E63"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64"/>
       <c r="B64"/>
       <c r="C64"/>
       <c r="D64"/>
       <c r="E64"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F64"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65"/>
       <c r="B65"/>
       <c r="C65"/>
       <c r="D65"/>
       <c r="E65"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F65"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66"/>
       <c r="B66"/>
       <c r="C66"/>
       <c r="D66"/>
       <c r="E66"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F66"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67"/>
       <c r="B67"/>
       <c r="C67"/>
       <c r="D67"/>
       <c r="E67"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F67"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68"/>
       <c r="B68"/>
       <c r="C68"/>
       <c r="D68"/>
       <c r="E68"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F68"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69"/>
       <c r="B69"/>
       <c r="C69"/>
       <c r="D69"/>
       <c r="E69"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F69"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70"/>
       <c r="B70"/>
       <c r="C70"/>
       <c r="D70"/>
       <c r="E70"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F70"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71"/>
       <c r="B71"/>
       <c r="C71"/>
       <c r="D71"/>
       <c r="E71"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F71"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72"/>
       <c r="B72"/>
       <c r="C72"/>
       <c r="D72"/>
       <c r="E72"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F72"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73"/>
       <c r="B73"/>
       <c r="C73"/>
       <c r="D73"/>
       <c r="E73"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F73"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74"/>
       <c r="B74"/>
       <c r="C74"/>
       <c r="D74"/>
       <c r="E74"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F74"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75"/>
       <c r="B75"/>
       <c r="C75"/>
       <c r="D75"/>
       <c r="E75"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F75"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76"/>
       <c r="B76"/>
       <c r="C76"/>
       <c r="D76"/>
       <c r="E76"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F76"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77"/>
       <c r="B77"/>
       <c r="C77"/>
       <c r="D77"/>
       <c r="E77"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F77"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78"/>
       <c r="B78"/>
       <c r="C78"/>
       <c r="D78"/>
       <c r="E78"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F78"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79"/>
       <c r="B79"/>
       <c r="C79"/>
       <c r="D79"/>
       <c r="E79"/>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F79"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80"/>
       <c r="B80"/>
       <c r="C80"/>
       <c r="D80"/>
       <c r="E80"/>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F80"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81"/>
       <c r="B81"/>
       <c r="C81"/>
       <c r="D81"/>
       <c r="E81"/>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F81"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82"/>
       <c r="B82"/>
       <c r="C82"/>
       <c r="D82"/>
       <c r="E82"/>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F82"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83"/>
       <c r="B83"/>
       <c r="C83"/>
       <c r="D83"/>
       <c r="E83"/>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F83"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84"/>
       <c r="B84"/>
       <c r="C84"/>
       <c r="D84"/>
       <c r="E84"/>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F84"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85"/>
       <c r="B85"/>
       <c r="C85"/>
       <c r="D85"/>
       <c r="E85"/>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F85"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86"/>
       <c r="B86"/>
       <c r="C86"/>
       <c r="D86"/>
       <c r="E86"/>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F86"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87"/>
       <c r="B87"/>
       <c r="C87"/>
       <c r="D87"/>
       <c r="E87"/>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F87"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88"/>
       <c r="B88"/>
       <c r="C88"/>
       <c r="D88"/>
       <c r="E88"/>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F88"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89"/>
       <c r="B89"/>
       <c r="C89"/>
       <c r="D89"/>
       <c r="E89"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F89"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90"/>
       <c r="B90"/>
       <c r="C90"/>
       <c r="D90"/>
       <c r="E90"/>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F90"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91"/>
       <c r="B91"/>
       <c r="C91"/>
       <c r="D91"/>
       <c r="E91"/>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F91"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92"/>
       <c r="B92"/>
       <c r="C92"/>
       <c r="D92"/>
       <c r="E92"/>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F92"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93"/>
       <c r="B93"/>
       <c r="C93"/>
       <c r="D93"/>
       <c r="E93"/>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F93"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94"/>
       <c r="B94"/>
       <c r="C94"/>
       <c r="D94"/>
       <c r="E94"/>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F94"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95"/>
       <c r="B95"/>
       <c r="C95"/>
       <c r="D95"/>
       <c r="E95"/>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F95"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96"/>
       <c r="B96"/>
       <c r="C96"/>
       <c r="D96"/>
       <c r="E96"/>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F96"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97"/>
       <c r="B97"/>
       <c r="C97"/>
       <c r="D97"/>
       <c r="E97"/>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F97"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98"/>
       <c r="B98"/>
       <c r="C98"/>
       <c r="D98"/>
       <c r="E98"/>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F98"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99"/>
       <c r="B99"/>
       <c r="C99"/>
       <c r="D99"/>
       <c r="E99"/>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F99"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100"/>
       <c r="B100"/>
       <c r="C100"/>
       <c r="D100"/>
       <c r="E100"/>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F100"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101"/>
       <c r="B101"/>
       <c r="C101"/>
       <c r="D101"/>
       <c r="E101"/>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F101"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102"/>
       <c r="B102"/>
       <c r="C102"/>
       <c r="D102"/>
       <c r="E102"/>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F102"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103"/>
       <c r="B103"/>
       <c r="C103"/>
       <c r="D103"/>
       <c r="E103"/>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F103"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104"/>
       <c r="B104"/>
       <c r="C104"/>
       <c r="D104"/>
       <c r="E104"/>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F104"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105"/>
       <c r="B105"/>
       <c r="C105"/>
       <c r="D105"/>
       <c r="E105"/>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F105"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106"/>
       <c r="B106"/>
       <c r="C106"/>
       <c r="D106"/>
       <c r="E106"/>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F106"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107"/>
       <c r="B107"/>
       <c r="C107"/>
       <c r="D107"/>
       <c r="E107"/>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F107"/>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108"/>
       <c r="B108"/>
       <c r="C108"/>
       <c r="D108"/>
       <c r="E108"/>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F108"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109"/>
       <c r="B109"/>
       <c r="C109"/>
       <c r="D109"/>
       <c r="E109"/>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F109"/>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110"/>
       <c r="B110"/>
       <c r="C110"/>
       <c r="D110"/>
       <c r="E110"/>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F110"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111"/>
       <c r="B111"/>
       <c r="C111"/>
       <c r="D111"/>
       <c r="E111"/>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F111"/>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112"/>
       <c r="B112"/>
       <c r="C112"/>
       <c r="D112"/>
       <c r="E112"/>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F112"/>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113"/>
       <c r="B113"/>
       <c r="C113"/>
       <c r="D113"/>
       <c r="E113"/>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F113"/>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114"/>
       <c r="B114"/>
       <c r="C114"/>
       <c r="D114"/>
       <c r="E114"/>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F114"/>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115"/>
       <c r="B115"/>
       <c r="C115"/>
       <c r="D115"/>
       <c r="E115"/>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F115"/>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116"/>
       <c r="B116"/>
       <c r="C116"/>
       <c r="D116"/>
       <c r="E116"/>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F116"/>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117"/>
       <c r="B117"/>
       <c r="C117"/>
       <c r="D117"/>
       <c r="E117"/>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F117"/>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118"/>
       <c r="B118"/>
       <c r="C118"/>
       <c r="D118"/>
       <c r="E118"/>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F118"/>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119"/>
       <c r="B119"/>
       <c r="C119"/>
       <c r="D119"/>
       <c r="E119"/>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F119"/>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120"/>
       <c r="B120"/>
       <c r="C120"/>
       <c r="D120"/>
       <c r="E120"/>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F120"/>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121"/>
       <c r="B121"/>
       <c r="C121"/>
       <c r="D121"/>
       <c r="E121"/>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F121"/>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122"/>
       <c r="B122"/>
       <c r="C122"/>
       <c r="D122"/>
       <c r="E122"/>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F122"/>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123"/>
       <c r="B123"/>
       <c r="C123"/>
       <c r="D123"/>
       <c r="E123"/>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F123"/>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124"/>
       <c r="B124"/>
       <c r="C124"/>
       <c r="D124"/>
       <c r="E124"/>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F124"/>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125"/>
       <c r="B125"/>
       <c r="C125"/>
       <c r="D125"/>
       <c r="E125"/>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F125"/>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126"/>
       <c r="B126"/>
       <c r="C126"/>
       <c r="D126"/>
       <c r="E126"/>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F126"/>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127"/>
       <c r="B127"/>
       <c r="C127"/>
       <c r="D127"/>
       <c r="E127"/>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F127"/>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128"/>
       <c r="B128"/>
       <c r="C128"/>
       <c r="D128"/>
       <c r="E128"/>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F128"/>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129"/>
       <c r="B129"/>
       <c r="C129"/>
       <c r="D129"/>
       <c r="E129"/>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F129"/>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130"/>
       <c r="B130"/>
       <c r="C130"/>
       <c r="D130"/>
       <c r="E130"/>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F130"/>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131"/>
       <c r="B131"/>
       <c r="C131"/>
       <c r="D131"/>
       <c r="E131"/>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F131"/>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132"/>
       <c r="B132"/>
       <c r="C132"/>
       <c r="D132"/>
       <c r="E132"/>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F132"/>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133"/>
       <c r="B133"/>
       <c r="C133"/>
       <c r="D133"/>
       <c r="E133"/>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F133"/>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134"/>
       <c r="B134"/>
       <c r="C134"/>
       <c r="D134"/>
       <c r="E134"/>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F134"/>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135"/>
       <c r="B135"/>
       <c r="C135"/>
       <c r="D135"/>
       <c r="E135"/>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F135"/>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136"/>
       <c r="B136"/>
       <c r="C136"/>
       <c r="D136"/>
       <c r="E136"/>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F136"/>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137"/>
       <c r="B137"/>
       <c r="C137"/>
       <c r="D137"/>
       <c r="E137"/>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F137"/>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138"/>
       <c r="B138"/>
       <c r="C138"/>
       <c r="D138"/>
       <c r="E138"/>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F138"/>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139"/>
       <c r="B139"/>
       <c r="C139"/>
       <c r="D139"/>
       <c r="E139"/>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F139"/>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140"/>
       <c r="B140"/>
       <c r="C140"/>
       <c r="D140"/>
       <c r="E140"/>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F140"/>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141"/>
       <c r="B141"/>
       <c r="C141"/>
       <c r="D141"/>
       <c r="E141"/>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F141"/>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142"/>
       <c r="B142"/>
       <c r="C142"/>
       <c r="D142"/>
       <c r="E142"/>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F142"/>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143"/>
       <c r="B143"/>
       <c r="C143"/>
       <c r="D143"/>
       <c r="E143"/>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F143"/>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144"/>
       <c r="B144"/>
       <c r="C144"/>
       <c r="D144"/>
       <c r="E144"/>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F144"/>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145"/>
       <c r="B145"/>
       <c r="C145"/>
       <c r="D145"/>
       <c r="E145"/>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F145"/>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146"/>
       <c r="B146"/>
       <c r="C146"/>
       <c r="D146"/>
       <c r="E146"/>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F146"/>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147"/>
       <c r="B147"/>
       <c r="C147"/>
       <c r="D147"/>
       <c r="E147"/>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F147"/>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148"/>
       <c r="B148"/>
       <c r="C148"/>
       <c r="D148"/>
       <c r="E148"/>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F148"/>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149"/>
       <c r="B149"/>
       <c r="C149"/>
       <c r="D149"/>
       <c r="E149"/>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F149"/>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150"/>
       <c r="B150"/>
       <c r="C150"/>
       <c r="D150"/>
       <c r="E150"/>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F150"/>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151"/>
       <c r="B151"/>
       <c r="C151"/>
       <c r="D151"/>
       <c r="E151"/>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F151"/>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152"/>
       <c r="B152"/>
       <c r="C152"/>
       <c r="D152"/>
       <c r="E152"/>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F152"/>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153"/>
       <c r="B153"/>
       <c r="C153"/>
       <c r="D153"/>
       <c r="E153"/>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F153"/>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154"/>
       <c r="B154"/>
       <c r="C154"/>
       <c r="D154"/>
       <c r="E154"/>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F154"/>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155"/>
       <c r="B155"/>
       <c r="C155"/>
       <c r="D155"/>
       <c r="E155"/>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F155"/>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156"/>
       <c r="B156"/>
       <c r="C156"/>
       <c r="D156"/>
       <c r="E156"/>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F156"/>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157"/>
       <c r="B157"/>
       <c r="C157"/>
       <c r="D157"/>
       <c r="E157"/>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F157"/>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158"/>
       <c r="B158"/>
       <c r="C158"/>
       <c r="D158"/>
       <c r="E158"/>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F158"/>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159"/>
       <c r="B159"/>
       <c r="C159"/>
       <c r="D159"/>
       <c r="E159"/>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F159"/>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160"/>
       <c r="B160"/>
       <c r="C160"/>
       <c r="D160"/>
       <c r="E160"/>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F160"/>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161"/>
       <c r="B161"/>
       <c r="C161"/>
       <c r="D161"/>
       <c r="E161"/>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F161"/>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162"/>
       <c r="B162"/>
       <c r="C162"/>
       <c r="D162"/>
       <c r="E162"/>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F162"/>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163"/>
       <c r="B163"/>
       <c r="C163"/>
       <c r="D163"/>
       <c r="E163"/>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F163"/>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164"/>
       <c r="B164"/>
       <c r="C164"/>
       <c r="D164"/>
       <c r="E164"/>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F164"/>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165"/>
       <c r="B165"/>
       <c r="C165"/>
       <c r="D165"/>
       <c r="E165"/>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F165"/>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166"/>
       <c r="B166"/>
       <c r="C166"/>
       <c r="D166"/>
       <c r="E166"/>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F166"/>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167"/>
       <c r="B167"/>
       <c r="C167"/>
       <c r="D167"/>
       <c r="E167"/>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F167"/>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168"/>
       <c r="B168"/>
       <c r="C168"/>
       <c r="D168"/>
       <c r="E168"/>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F168"/>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169"/>
       <c r="B169"/>
       <c r="C169"/>
       <c r="D169"/>
       <c r="E169"/>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F169"/>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170"/>
       <c r="B170"/>
       <c r="C170"/>
       <c r="D170"/>
       <c r="E170"/>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F170"/>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171"/>
       <c r="B171"/>
       <c r="C171"/>
       <c r="D171"/>
       <c r="E171"/>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F171"/>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172"/>
       <c r="B172"/>
       <c r="C172"/>
       <c r="D172"/>
       <c r="E172"/>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F172"/>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173"/>
       <c r="B173"/>
       <c r="C173"/>
       <c r="D173"/>
       <c r="E173"/>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F173"/>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174"/>
       <c r="B174"/>
       <c r="C174"/>
       <c r="D174"/>
       <c r="E174"/>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F174"/>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175"/>
       <c r="B175"/>
       <c r="C175"/>
       <c r="D175"/>
       <c r="E175"/>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F175"/>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176"/>
       <c r="B176"/>
       <c r="C176"/>
       <c r="D176"/>
       <c r="E176"/>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F176"/>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177"/>
       <c r="B177"/>
       <c r="C177"/>
       <c r="D177"/>
       <c r="E177"/>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F177"/>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178"/>
       <c r="B178"/>
       <c r="C178"/>
       <c r="D178"/>
       <c r="E178"/>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F178"/>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179"/>
       <c r="B179"/>
       <c r="C179"/>
       <c r="D179"/>
       <c r="E179"/>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F179"/>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180"/>
       <c r="B180"/>
       <c r="C180"/>
       <c r="D180"/>
       <c r="E180"/>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F180"/>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181"/>
       <c r="B181"/>
       <c r="C181"/>
       <c r="D181"/>
       <c r="E181"/>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F181"/>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182"/>
       <c r="B182"/>
       <c r="C182"/>
       <c r="D182"/>
       <c r="E182"/>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F182"/>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183"/>
       <c r="B183"/>
       <c r="C183"/>
       <c r="D183"/>
       <c r="E183"/>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F183"/>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184"/>
       <c r="B184"/>
       <c r="C184"/>
       <c r="D184"/>
       <c r="E184"/>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F184"/>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185"/>
       <c r="B185"/>
       <c r="C185"/>
       <c r="D185"/>
       <c r="E185"/>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F185"/>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186"/>
       <c r="B186"/>
       <c r="C186"/>
       <c r="D186"/>
       <c r="E186"/>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F186"/>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187"/>
       <c r="B187"/>
       <c r="C187"/>
       <c r="D187"/>
       <c r="E187"/>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F187"/>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188"/>
       <c r="B188"/>
       <c r="C188"/>
       <c r="D188"/>
       <c r="E188"/>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F188"/>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189"/>
       <c r="B189"/>
       <c r="C189"/>
       <c r="D189"/>
       <c r="E189"/>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F189"/>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190"/>
       <c r="B190"/>
       <c r="C190"/>
       <c r="D190"/>
       <c r="E190"/>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F190"/>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191"/>
       <c r="B191"/>
       <c r="C191"/>
       <c r="D191"/>
       <c r="E191"/>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F191"/>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192"/>
       <c r="B192"/>
       <c r="C192"/>
       <c r="D192"/>
       <c r="E192"/>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F192"/>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193"/>
       <c r="B193"/>
       <c r="C193"/>
       <c r="D193"/>
       <c r="E193"/>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F193"/>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194"/>
       <c r="B194"/>
       <c r="C194"/>
       <c r="D194"/>
       <c r="E194"/>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F194"/>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195"/>
       <c r="B195"/>
       <c r="C195"/>
       <c r="D195"/>
       <c r="E195"/>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F195"/>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196"/>
       <c r="B196"/>
       <c r="C196"/>
       <c r="D196"/>
       <c r="E196"/>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F196"/>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197"/>
       <c r="B197"/>
       <c r="C197"/>
       <c r="D197"/>
       <c r="E197"/>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F197"/>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198"/>
       <c r="B198"/>
       <c r="C198"/>
       <c r="D198"/>
       <c r="E198"/>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F198"/>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199"/>
       <c r="B199"/>
       <c r="C199"/>
       <c r="D199"/>
       <c r="E199"/>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F199"/>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200"/>
       <c r="B200"/>
       <c r="C200"/>
       <c r="D200"/>
       <c r="E200"/>
-    </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F200"/>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201"/>
       <c r="B201"/>
       <c r="C201"/>
       <c r="D201"/>
       <c r="E201"/>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F201"/>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A202"/>
       <c r="B202"/>
       <c r="C202"/>
       <c r="D202"/>
       <c r="E202"/>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F202"/>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A203"/>
       <c r="B203"/>
       <c r="C203"/>
       <c r="D203"/>
       <c r="E203"/>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F203"/>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A204"/>
       <c r="B204"/>
       <c r="C204"/>
       <c r="D204"/>
       <c r="E204"/>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F204"/>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A205"/>
       <c r="B205"/>
       <c r="C205"/>
       <c r="D205"/>
       <c r="E205"/>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F205"/>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A206"/>
       <c r="B206"/>
       <c r="C206"/>
       <c r="D206"/>
       <c r="E206"/>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F206"/>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A207"/>
       <c r="B207"/>
       <c r="C207"/>
       <c r="D207"/>
       <c r="E207"/>
-    </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F207"/>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A208"/>
       <c r="B208"/>
       <c r="C208"/>
       <c r="D208"/>
       <c r="E208"/>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F208"/>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A209"/>
       <c r="B209"/>
       <c r="C209"/>
       <c r="D209"/>
       <c r="E209"/>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F209"/>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A210"/>
       <c r="B210"/>
       <c r="C210"/>
       <c r="D210"/>
       <c r="E210"/>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F210"/>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A211"/>
       <c r="B211"/>
       <c r="C211"/>
       <c r="D211"/>
       <c r="E211"/>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F211"/>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A212"/>
       <c r="B212"/>
       <c r="C212"/>
       <c r="D212"/>
       <c r="E212"/>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F212"/>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A213"/>
       <c r="B213"/>
       <c r="C213"/>
       <c r="D213"/>
       <c r="E213"/>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F213"/>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A214"/>
       <c r="B214"/>
       <c r="C214"/>
       <c r="D214"/>
       <c r="E214"/>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F214"/>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A215"/>
       <c r="B215"/>
       <c r="C215"/>
       <c r="D215"/>
       <c r="E215"/>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F215"/>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A216"/>
       <c r="B216"/>
       <c r="C216"/>
       <c r="D216"/>
       <c r="E216"/>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F216"/>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A217"/>
       <c r="B217"/>
       <c r="C217"/>
       <c r="D217"/>
       <c r="E217"/>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F217"/>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A218"/>
       <c r="B218"/>
       <c r="C218"/>
       <c r="D218"/>
       <c r="E218"/>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F218"/>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A219"/>
       <c r="B219"/>
       <c r="C219"/>
       <c r="D219"/>
       <c r="E219"/>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F219"/>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A220"/>
       <c r="B220"/>
       <c r="C220"/>
       <c r="D220"/>
       <c r="E220"/>
-    </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F220"/>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A221"/>
       <c r="B221"/>
       <c r="C221"/>
       <c r="D221"/>
       <c r="E221"/>
-    </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F221"/>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A222"/>
       <c r="B222"/>
       <c r="C222"/>
       <c r="D222"/>
       <c r="E222"/>
-    </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F222"/>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A223"/>
       <c r="B223"/>
       <c r="C223"/>
       <c r="D223"/>
       <c r="E223"/>
-    </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F223"/>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A224"/>
       <c r="B224"/>
       <c r="C224"/>
       <c r="D224"/>
       <c r="E224"/>
-    </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F224"/>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A225"/>
       <c r="B225"/>
       <c r="C225"/>
       <c r="D225"/>
       <c r="E225"/>
-    </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F225"/>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A226"/>
       <c r="B226"/>
       <c r="C226"/>
       <c r="D226"/>
       <c r="E226"/>
-    </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F226"/>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A227"/>
       <c r="B227"/>
       <c r="C227"/>
       <c r="D227"/>
       <c r="E227"/>
-    </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F227"/>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A228"/>
       <c r="B228"/>
       <c r="C228"/>
       <c r="D228"/>
       <c r="E228"/>
-    </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F228"/>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A229"/>
       <c r="B229"/>
       <c r="C229"/>
       <c r="D229"/>
       <c r="E229"/>
-    </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F229"/>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A230"/>
       <c r="B230"/>
       <c r="C230"/>
       <c r="D230"/>
       <c r="E230"/>
-    </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F230"/>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A231"/>
       <c r="B231"/>
       <c r="C231"/>
       <c r="D231"/>
       <c r="E231"/>
-    </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F231"/>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A232"/>
       <c r="B232"/>
       <c r="C232"/>
       <c r="D232"/>
       <c r="E232"/>
-    </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F232"/>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A233"/>
       <c r="B233"/>
       <c r="C233"/>
       <c r="D233"/>
       <c r="E233"/>
-    </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F233"/>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A234"/>
       <c r="B234"/>
       <c r="C234"/>
       <c r="D234"/>
       <c r="E234"/>
-    </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F234"/>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A235"/>
       <c r="B235"/>
       <c r="C235"/>
       <c r="D235"/>
       <c r="E235"/>
-    </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F235"/>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A236"/>
       <c r="B236"/>
       <c r="C236"/>
       <c r="D236"/>
       <c r="E236"/>
-    </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F236"/>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A237"/>
       <c r="B237"/>
       <c r="C237"/>
       <c r="D237"/>
       <c r="E237"/>
-    </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F237"/>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A238"/>
       <c r="B238"/>
       <c r="C238"/>
       <c r="D238"/>
       <c r="E238"/>
-    </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F238"/>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A239"/>
       <c r="B239"/>
       <c r="C239"/>
       <c r="D239"/>
       <c r="E239"/>
-    </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F239"/>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A240"/>
       <c r="B240"/>
       <c r="C240"/>
       <c r="D240"/>
       <c r="E240"/>
-    </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F240"/>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A241"/>
       <c r="B241"/>
       <c r="C241"/>
       <c r="D241"/>
       <c r="E241"/>
-    </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F241"/>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A242"/>
       <c r="B242"/>
       <c r="C242"/>
       <c r="D242"/>
       <c r="E242"/>
-    </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F242"/>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A243"/>
       <c r="B243"/>
       <c r="C243"/>
       <c r="D243"/>
       <c r="E243"/>
-    </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F243"/>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A244"/>
       <c r="B244"/>
       <c r="C244"/>
       <c r="D244"/>
       <c r="E244"/>
-    </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F244"/>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A245"/>
       <c r="B245"/>
       <c r="C245"/>
       <c r="D245"/>
       <c r="E245"/>
-    </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F245"/>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A246"/>
       <c r="B246"/>
       <c r="C246"/>
       <c r="D246"/>
       <c r="E246"/>
-    </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F246"/>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A247"/>
       <c r="B247"/>
       <c r="C247"/>
       <c r="D247"/>
       <c r="E247"/>
-    </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F247"/>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A248"/>
       <c r="B248"/>
       <c r="C248"/>
       <c r="D248"/>
       <c r="E248"/>
-    </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F248"/>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A249"/>
       <c r="B249"/>
       <c r="C249"/>
       <c r="D249"/>
       <c r="E249"/>
-    </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F249"/>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A250"/>
       <c r="B250"/>
       <c r="C250"/>
       <c r="D250"/>
       <c r="E250"/>
-    </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F250"/>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A251"/>
       <c r="B251"/>
       <c r="C251"/>
       <c r="D251"/>
       <c r="E251"/>
-    </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F251"/>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A252"/>
       <c r="B252"/>
       <c r="C252"/>
       <c r="D252"/>
       <c r="E252"/>
-    </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F252"/>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A253"/>
       <c r="B253"/>
       <c r="C253"/>
       <c r="D253"/>
       <c r="E253"/>
-    </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F253"/>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A254"/>
       <c r="B254"/>
       <c r="C254"/>
       <c r="D254"/>
       <c r="E254"/>
-    </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F254"/>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A255"/>
       <c r="B255"/>
       <c r="C255"/>
       <c r="D255"/>
       <c r="E255"/>
-    </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F255"/>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A256"/>
       <c r="B256"/>
       <c r="C256"/>
       <c r="D256"/>
       <c r="E256"/>
-    </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F256"/>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A257"/>
       <c r="B257"/>
       <c r="C257"/>
       <c r="D257"/>
       <c r="E257"/>
-    </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F257"/>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A258"/>
       <c r="B258"/>
       <c r="C258"/>
       <c r="D258"/>
       <c r="E258"/>
-    </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F258"/>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A259"/>
       <c r="B259"/>
       <c r="C259"/>
       <c r="D259"/>
       <c r="E259"/>
-    </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F259"/>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A260"/>
       <c r="B260"/>
       <c r="C260"/>
       <c r="D260"/>
       <c r="E260"/>
-    </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F260"/>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A261"/>
       <c r="B261"/>
       <c r="C261"/>
       <c r="D261"/>
       <c r="E261"/>
-    </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F261"/>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A262"/>
       <c r="B262"/>
       <c r="C262"/>
       <c r="D262"/>
       <c r="E262"/>
-    </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F262"/>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A263"/>
       <c r="B263"/>
       <c r="C263"/>
       <c r="D263"/>
       <c r="E263"/>
-    </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F263"/>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A264"/>
       <c r="B264"/>
       <c r="C264"/>
       <c r="D264"/>
       <c r="E264"/>
-    </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F264"/>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A265"/>
       <c r="B265"/>
       <c r="C265"/>
       <c r="D265"/>
       <c r="E265"/>
-    </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F265"/>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A266"/>
       <c r="B266"/>
       <c r="C266"/>
       <c r="D266"/>
       <c r="E266"/>
-    </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F266"/>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A267"/>
       <c r="B267"/>
       <c r="C267"/>
       <c r="D267"/>
       <c r="E267"/>
-    </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F267"/>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A268"/>
       <c r="B268"/>
       <c r="C268"/>
       <c r="D268"/>
       <c r="E268"/>
-    </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F268"/>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A269"/>
       <c r="B269"/>
       <c r="C269"/>
       <c r="D269"/>
       <c r="E269"/>
-    </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F269"/>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A270"/>
       <c r="B270"/>
       <c r="C270"/>
       <c r="D270"/>
       <c r="E270"/>
-    </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F270"/>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A271"/>
       <c r="B271"/>
       <c r="C271"/>
       <c r="D271"/>
       <c r="E271"/>
-    </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F271"/>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A272"/>
       <c r="B272"/>
       <c r="C272"/>
       <c r="D272"/>
       <c r="E272"/>
-    </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F272"/>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A273"/>
       <c r="B273"/>
       <c r="C273"/>
       <c r="D273"/>
       <c r="E273"/>
-    </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F273"/>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A274"/>
       <c r="B274"/>
       <c r="C274"/>
       <c r="D274"/>
       <c r="E274"/>
-    </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F274"/>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A275"/>
       <c r="B275"/>
       <c r="C275"/>
       <c r="D275"/>
       <c r="E275"/>
-    </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F275"/>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A276"/>
       <c r="B276"/>
       <c r="C276"/>
       <c r="D276"/>
       <c r="E276"/>
-    </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F276"/>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A277"/>
       <c r="B277"/>
       <c r="C277"/>
       <c r="D277"/>
       <c r="E277"/>
-    </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F277"/>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A278"/>
       <c r="B278"/>
       <c r="C278"/>
       <c r="D278"/>
       <c r="E278"/>
-    </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F278"/>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A279"/>
       <c r="B279"/>
       <c r="C279"/>
       <c r="D279"/>
       <c r="E279"/>
-    </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F279"/>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A280"/>
       <c r="B280"/>
       <c r="C280"/>
       <c r="D280"/>
       <c r="E280"/>
-    </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F280"/>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A281"/>
       <c r="B281"/>
       <c r="C281"/>
       <c r="D281"/>
       <c r="E281"/>
-    </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F281"/>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A282"/>
       <c r="B282"/>
       <c r="C282"/>
       <c r="D282"/>
       <c r="E282"/>
-    </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F282"/>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A283"/>
       <c r="B283"/>
       <c r="C283"/>
       <c r="D283"/>
       <c r="E283"/>
-    </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F283"/>
+    </row>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A284"/>
       <c r="B284"/>
       <c r="C284"/>
       <c r="D284"/>
       <c r="E284"/>
-    </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F284"/>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A285"/>
       <c r="B285"/>
       <c r="C285"/>
       <c r="D285"/>
       <c r="E285"/>
-    </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F285"/>
+    </row>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A286"/>
       <c r="B286"/>
       <c r="C286"/>
       <c r="D286"/>
       <c r="E286"/>
-    </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F286"/>
+    </row>
+    <row r="287" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A287"/>
       <c r="B287"/>
       <c r="C287"/>
       <c r="D287"/>
       <c r="E287"/>
-    </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F287"/>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A288"/>
       <c r="B288"/>
       <c r="C288"/>
       <c r="D288"/>
       <c r="E288"/>
-    </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F288"/>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A289"/>
       <c r="B289"/>
       <c r="C289"/>
       <c r="D289"/>
       <c r="E289"/>
-    </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F289"/>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A290"/>
       <c r="B290"/>
       <c r="C290"/>
       <c r="D290"/>
       <c r="E290"/>
-    </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F290"/>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A291"/>
       <c r="B291"/>
       <c r="C291"/>
       <c r="D291"/>
       <c r="E291"/>
-    </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F291"/>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A292"/>
       <c r="B292"/>
       <c r="C292"/>
       <c r="D292"/>
       <c r="E292"/>
-    </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F292"/>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A293"/>
       <c r="B293"/>
       <c r="C293"/>
       <c r="D293"/>
       <c r="E293"/>
-    </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F293"/>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A294"/>
       <c r="B294"/>
       <c r="C294"/>
       <c r="D294"/>
       <c r="E294"/>
-    </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F294"/>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A295"/>
       <c r="B295"/>
       <c r="C295"/>
       <c r="D295"/>
       <c r="E295"/>
-    </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F295"/>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A296"/>
       <c r="B296"/>
       <c r="C296"/>
       <c r="D296"/>
       <c r="E296"/>
-    </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F296"/>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A297"/>
       <c r="B297"/>
       <c r="C297"/>
       <c r="D297"/>
       <c r="E297"/>
-    </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F297"/>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A298"/>
       <c r="B298"/>
       <c r="C298"/>
       <c r="D298"/>
       <c r="E298"/>
-    </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F298"/>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A299"/>
       <c r="B299"/>
       <c r="C299"/>
       <c r="D299"/>
       <c r="E299"/>
-    </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F299"/>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A300"/>
       <c r="B300"/>
       <c r="C300"/>
       <c r="D300"/>
       <c r="E300"/>
-    </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F300"/>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A301"/>
       <c r="B301"/>
       <c r="C301"/>
       <c r="D301"/>
       <c r="E301"/>
-    </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F301"/>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A302"/>
       <c r="B302"/>
       <c r="C302"/>
       <c r="D302"/>
       <c r="E302"/>
-    </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F302"/>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A303"/>
       <c r="B303"/>
       <c r="C303"/>
       <c r="D303"/>
       <c r="E303"/>
-    </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F303"/>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A304"/>
       <c r="B304"/>
       <c r="C304"/>
       <c r="D304"/>
       <c r="E304"/>
-    </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F304"/>
+    </row>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A305"/>
       <c r="B305"/>
       <c r="C305"/>
       <c r="D305"/>
       <c r="E305"/>
+      <c r="F305"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Check of Groups and Strategies
</commit_message>
<xml_diff>
--- a/inst/models/checkimab/model.xlsx
+++ b/inst/models/checkimab/model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexander_lonshteyn/Desktop/HeRomod2/heRomod2/inst/models/checkimab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E85240E-D006-094B-864C-FA47109FE762}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABFCFC8-AD8C-1C47-82A4-27124B5C4D29}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="740" windowWidth="22240" windowHeight="13580" activeTab="6" xr2:uid="{F2154858-BAC7-AB46-9308-23215F5D2873}"/>
+    <workbookView xWindow="1740" yWindow="780" windowWidth="22240" windowHeight="13580" firstSheet="2" activeTab="2" xr2:uid="{F2154858-BAC7-AB46-9308-23215F5D2873}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -11687,8 +11687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4FC5599-9A38-1A41-A80E-4A51D6E0BF6E}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11801,7 +11801,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16492,7 +16492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F0D78FB-8401-9E4C-9EB5-A7C336F3C948}">
   <dimension ref="A1:F305"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>

</xml_diff>